<commit_message>
Update new map file for PLC. (From Tong)
</commit_message>
<xml_diff>
--- a/MemoryMap/NI.xlsx
+++ b/MemoryMap/NI.xlsx
@@ -850,7 +850,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q168" authorId="0">
+    <comment ref="Q169" authorId="0">
       <text>
         <r>
           <rPr>
@@ -866,7 +866,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q169" authorId="0">
+    <comment ref="Q170" authorId="0">
       <text>
         <r>
           <rPr>
@@ -881,7 +881,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q170" authorId="0">
+    <comment ref="Q171" authorId="0">
       <text>
         <r>
           <rPr>
@@ -897,7 +897,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q171" authorId="0">
+    <comment ref="Q172" authorId="0">
       <text>
         <r>
           <rPr>
@@ -912,7 +912,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S182" authorId="0">
+    <comment ref="S183" authorId="0">
       <text>
         <r>
           <rPr>
@@ -939,7 +939,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q193" authorId="0">
+    <comment ref="Q196" authorId="0">
       <text>
         <r>
           <rPr>
@@ -955,7 +955,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q194" authorId="0">
+    <comment ref="Q197" authorId="0">
       <text>
         <r>
           <rPr>
@@ -970,7 +970,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q195" authorId="0">
+    <comment ref="Q198" authorId="0">
       <text>
         <r>
           <rPr>
@@ -986,7 +986,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q196" authorId="0">
+    <comment ref="Q199" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1006,7 +1006,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="211">
   <si>
     <t>Device name</t>
   </si>
@@ -1624,13 +1624,28 @@
   </si>
   <si>
     <t>M4212</t>
+  </si>
+  <si>
+    <t>D8338</t>
+  </si>
+  <si>
+    <t>CAMERA NO.</t>
+  </si>
+  <si>
+    <t>D8310</t>
+  </si>
+  <si>
+    <t>D8339</t>
+  </si>
+  <si>
+    <t>PRODUCT PLAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1686,8 +1701,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1727,6 +1749,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1853,7 +1881,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1893,6 +1921,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1926,11 +1957,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3794,13 +3824,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>167</xdr:row>
+      <xdr:row>168</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>167</xdr:row>
+      <xdr:row>168</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3845,13 +3875,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>169</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>169</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3896,13 +3926,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>170</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>170</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3947,13 +3977,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>170</xdr:row>
+      <xdr:row>171</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>170</xdr:row>
+      <xdr:row>171</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3998,13 +4028,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>192</xdr:row>
+      <xdr:row>195</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>192</xdr:row>
+      <xdr:row>195</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4049,13 +4079,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>193</xdr:row>
+      <xdr:row>196</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>193</xdr:row>
+      <xdr:row>196</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4100,13 +4130,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>194</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>194</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4151,13 +4181,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>195</xdr:row>
+      <xdr:row>198</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>195</xdr:row>
+      <xdr:row>198</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4486,17 +4516,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:X196"/>
+  <dimension ref="A2:X199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="V182" sqref="V182"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="A171" sqref="A171:XFD171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="17" width="4.7109375" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" customWidth="1"/>
     <col min="20" max="20" width="10.85546875" customWidth="1"/>
     <col min="22" max="22" width="20.140625" customWidth="1"/>
     <col min="23" max="23" width="11.7109375" customWidth="1"/>
@@ -4597,7 +4627,7 @@
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
-      <c r="R4" s="23" t="s">
+      <c r="R4" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S4" s="9" t="s">
@@ -4624,7 +4654,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
-      <c r="R5" s="23"/>
+      <c r="R5" s="26"/>
       <c r="S5" s="9">
         <v>23</v>
       </c>
@@ -4649,7 +4679,7 @@
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
-      <c r="R6" s="23"/>
+      <c r="R6" s="26"/>
       <c r="S6" s="9">
         <v>45</v>
       </c>
@@ -4674,7 +4704,7 @@
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="23"/>
+      <c r="R7" s="26"/>
       <c r="S7" s="9">
         <v>6</v>
       </c>
@@ -4699,7 +4729,7 @@
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="23"/>
+      <c r="R8" s="26"/>
     </row>
     <row r="9" spans="1:21" ht="18.75" customHeight="1">
       <c r="A9" s="6" t="s">
@@ -4721,7 +4751,7 @@
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="23"/>
+      <c r="R9" s="26"/>
     </row>
     <row r="10" spans="1:21" ht="18.75" customHeight="1">
       <c r="A10" s="6" t="s">
@@ -4743,7 +4773,7 @@
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
-      <c r="R10" s="23"/>
+      <c r="R10" s="26"/>
       <c r="S10" t="s">
         <v>17</v>
       </c>
@@ -4768,11 +4798,11 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
-      <c r="R11" s="23"/>
+      <c r="R11" s="26"/>
       <c r="S11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T11" s="29" t="s">
+      <c r="T11" s="32" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4802,7 +4832,7 @@
       <c r="S12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T12" s="30"/>
+      <c r="T12" s="33"/>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="6" t="s">
@@ -4830,7 +4860,7 @@
       <c r="S13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T13" s="30"/>
+      <c r="T13" s="33"/>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="6" t="s">
@@ -4858,7 +4888,7 @@
       <c r="S14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T14" s="30"/>
+      <c r="T14" s="33"/>
       <c r="U14" t="s">
         <v>28</v>
       </c>
@@ -4889,7 +4919,7 @@
       <c r="S15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T15" s="30"/>
+      <c r="T15" s="33"/>
       <c r="U15" t="s">
         <v>30</v>
       </c>
@@ -4920,7 +4950,7 @@
       <c r="S16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T16" s="30"/>
+      <c r="T16" s="33"/>
       <c r="U16" t="s">
         <v>32</v>
       </c>
@@ -4949,7 +4979,7 @@
         <v>27</v>
       </c>
       <c r="S17" s="6"/>
-      <c r="T17" s="31"/>
+      <c r="T17" s="34"/>
       <c r="U17" t="s">
         <v>34</v>
       </c>
@@ -5030,13 +5060,13 @@
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
-      <c r="R21" s="23" t="s">
+      <c r="R21" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S21" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T21" s="28" t="s">
+      <c r="T21" s="31" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5060,11 +5090,11 @@
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
-      <c r="R22" s="23"/>
+      <c r="R22" s="26"/>
       <c r="S22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T22" s="28"/>
+      <c r="T22" s="31"/>
     </row>
     <row r="23" spans="1:21" ht="15" customHeight="1">
       <c r="A23" s="6" t="s">
@@ -5086,9 +5116,9 @@
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
-      <c r="R23" s="23"/>
+      <c r="R23" s="26"/>
       <c r="S23" s="15"/>
-      <c r="T23" s="28"/>
+      <c r="T23" s="31"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1">
       <c r="A24" s="6" t="s">
@@ -5110,11 +5140,11 @@
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
-      <c r="R24" s="23"/>
+      <c r="R24" s="26"/>
       <c r="S24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T24" s="28"/>
+      <c r="T24" s="31"/>
     </row>
     <row r="25" spans="1:21" ht="15" customHeight="1">
       <c r="A25" s="6" t="s">
@@ -5136,11 +5166,11 @@
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
-      <c r="R25" s="23"/>
+      <c r="R25" s="26"/>
       <c r="S25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T25" s="28"/>
+      <c r="T25" s="31"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" customHeight="1">
       <c r="A26" s="6" t="s">
@@ -5162,11 +5192,11 @@
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
-      <c r="R26" s="23"/>
+      <c r="R26" s="26"/>
       <c r="S26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T26" s="28"/>
+      <c r="T26" s="31"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" customHeight="1">
       <c r="A27" s="6" t="s">
@@ -5188,11 +5218,11 @@
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
-      <c r="R27" s="23"/>
+      <c r="R27" s="26"/>
       <c r="S27" t="s">
         <v>17</v>
       </c>
-      <c r="T27" s="28"/>
+      <c r="T27" s="31"/>
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="6" t="s">
@@ -5214,11 +5244,11 @@
       <c r="O28" s="17"/>
       <c r="P28" s="17"/>
       <c r="Q28" s="17"/>
-      <c r="R28" s="23"/>
+      <c r="R28" s="26"/>
       <c r="S28" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T28" s="28"/>
+      <c r="T28" s="31"/>
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="6" t="s">
@@ -5244,7 +5274,7 @@
         <v>22</v>
       </c>
       <c r="S29" s="6"/>
-      <c r="T29" s="28"/>
+      <c r="T29" s="31"/>
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="6" t="s">
@@ -5270,7 +5300,7 @@
         <v>25</v>
       </c>
       <c r="S30" s="6"/>
-      <c r="T30" s="28"/>
+      <c r="T30" s="31"/>
     </row>
     <row r="31" spans="1:21" ht="15" customHeight="1">
       <c r="A31" s="6" t="s">
@@ -5298,7 +5328,7 @@
       <c r="S31" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T31" s="28"/>
+      <c r="T31" s="31"/>
       <c r="U31" t="s">
         <v>28</v>
       </c>
@@ -5329,7 +5359,7 @@
       <c r="S32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T32" s="28"/>
+      <c r="T32" s="31"/>
       <c r="U32" t="s">
         <v>30</v>
       </c>
@@ -5360,7 +5390,7 @@
       <c r="S33" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T33" s="28"/>
+      <c r="T33" s="31"/>
       <c r="U33" t="s">
         <v>32</v>
       </c>
@@ -5391,7 +5421,7 @@
       <c r="S34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T34" s="28"/>
+      <c r="T34" s="31"/>
       <c r="U34" t="s">
         <v>34</v>
       </c>
@@ -5512,11 +5542,11 @@
       <c r="O38" s="8"/>
       <c r="P38" s="8"/>
       <c r="Q38" s="8"/>
-      <c r="R38" s="23" t="s">
+      <c r="R38" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S38" s="6"/>
-      <c r="T38" s="32" t="s">
+      <c r="T38" s="35" t="s">
         <v>51</v>
       </c>
     </row>
@@ -5540,9 +5570,9 @@
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
       <c r="Q39" s="8"/>
-      <c r="R39" s="23"/>
+      <c r="R39" s="26"/>
       <c r="S39" s="6"/>
-      <c r="T39" s="33"/>
+      <c r="T39" s="36"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" customHeight="1">
       <c r="A40" s="6" t="s">
@@ -5564,9 +5594,9 @@
       <c r="O40" s="8"/>
       <c r="P40" s="8"/>
       <c r="Q40" s="8"/>
-      <c r="R40" s="23"/>
+      <c r="R40" s="26"/>
       <c r="S40" s="15"/>
-      <c r="T40" s="33"/>
+      <c r="T40" s="36"/>
     </row>
     <row r="41" spans="1:21" ht="15.75" customHeight="1">
       <c r="A41" s="6" t="s">
@@ -5588,9 +5618,9 @@
       <c r="O41" s="8"/>
       <c r="P41" s="8"/>
       <c r="Q41" s="8"/>
-      <c r="R41" s="23"/>
+      <c r="R41" s="26"/>
       <c r="S41" s="15"/>
-      <c r="T41" s="33"/>
+      <c r="T41" s="36"/>
     </row>
     <row r="42" spans="1:21" ht="15.75" customHeight="1">
       <c r="A42" s="6" t="s">
@@ -5612,9 +5642,9 @@
       <c r="O42" s="8"/>
       <c r="P42" s="8"/>
       <c r="Q42" s="8"/>
-      <c r="R42" s="23"/>
+      <c r="R42" s="26"/>
       <c r="S42" s="15"/>
-      <c r="T42" s="33"/>
+      <c r="T42" s="36"/>
     </row>
     <row r="43" spans="1:21" ht="15.75" customHeight="1">
       <c r="A43" s="6" t="s">
@@ -5636,9 +5666,9 @@
       <c r="O43" s="8"/>
       <c r="P43" s="8"/>
       <c r="Q43" s="8"/>
-      <c r="R43" s="23"/>
+      <c r="R43" s="26"/>
       <c r="S43" s="15"/>
-      <c r="T43" s="33"/>
+      <c r="T43" s="36"/>
     </row>
     <row r="44" spans="1:21" ht="15.75" customHeight="1">
       <c r="A44" s="6" t="s">
@@ -5660,11 +5690,11 @@
       <c r="O44" s="8"/>
       <c r="P44" s="8"/>
       <c r="Q44" s="8"/>
-      <c r="R44" s="23"/>
+      <c r="R44" s="26"/>
       <c r="S44" t="s">
         <v>17</v>
       </c>
-      <c r="T44" s="33"/>
+      <c r="T44" s="36"/>
     </row>
     <row r="45" spans="1:21" ht="15" customHeight="1">
       <c r="A45" s="6" t="s">
@@ -5686,11 +5716,11 @@
       <c r="O45" s="17"/>
       <c r="P45" s="17"/>
       <c r="Q45" s="17"/>
-      <c r="R45" s="23"/>
+      <c r="R45" s="26"/>
       <c r="S45" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T45" s="33"/>
+      <c r="T45" s="36"/>
     </row>
     <row r="46" spans="1:21" ht="15" customHeight="1">
       <c r="A46" s="6" t="s">
@@ -5718,7 +5748,7 @@
       <c r="S46" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T46" s="33"/>
+      <c r="T46" s="36"/>
     </row>
     <row r="47" spans="1:21" ht="15" customHeight="1">
       <c r="A47" s="6" t="s">
@@ -5746,7 +5776,7 @@
       <c r="S47" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T47" s="33"/>
+      <c r="T47" s="36"/>
     </row>
     <row r="48" spans="1:21" ht="15" customHeight="1">
       <c r="A48" s="6" t="s">
@@ -5774,7 +5804,7 @@
       <c r="S48" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T48" s="33"/>
+      <c r="T48" s="36"/>
       <c r="U48" t="s">
         <v>28</v>
       </c>
@@ -5805,7 +5835,7 @@
       <c r="S49" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T49" s="33"/>
+      <c r="T49" s="36"/>
       <c r="U49" t="s">
         <v>30</v>
       </c>
@@ -5836,7 +5866,7 @@
       <c r="S50" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T50" s="33"/>
+      <c r="T50" s="36"/>
       <c r="U50" t="s">
         <v>32</v>
       </c>
@@ -5867,7 +5897,7 @@
       <c r="S51" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T51" s="33"/>
+      <c r="T51" s="36"/>
       <c r="U51" t="s">
         <v>34</v>
       </c>
@@ -5928,7 +5958,7 @@
         <v>7</v>
       </c>
       <c r="S54" s="6"/>
-      <c r="T54" s="28" t="s">
+      <c r="T54" s="31" t="s">
         <v>65</v>
       </c>
       <c r="W54" s="20" t="s">
@@ -5958,11 +5988,11 @@
       <c r="O55" s="8"/>
       <c r="P55" s="8"/>
       <c r="Q55" s="8"/>
-      <c r="R55" s="23" t="s">
+      <c r="R55" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S55" s="6"/>
-      <c r="T55" s="28"/>
+      <c r="T55" s="31"/>
       <c r="W55" s="20">
         <v>2</v>
       </c>
@@ -5990,9 +6020,9 @@
       <c r="O56" s="8"/>
       <c r="P56" s="8"/>
       <c r="Q56" s="8"/>
-      <c r="R56" s="23"/>
+      <c r="R56" s="26"/>
       <c r="S56" s="6"/>
-      <c r="T56" s="28"/>
+      <c r="T56" s="31"/>
       <c r="W56" s="20">
         <v>3</v>
       </c>
@@ -6020,9 +6050,9 @@
       <c r="O57" s="8"/>
       <c r="P57" s="8"/>
       <c r="Q57" s="8"/>
-      <c r="R57" s="23"/>
+      <c r="R57" s="26"/>
       <c r="S57" s="6"/>
-      <c r="T57" s="28"/>
+      <c r="T57" s="31"/>
       <c r="W57" s="20">
         <v>4</v>
       </c>
@@ -6050,9 +6080,9 @@
       <c r="O58" s="8"/>
       <c r="P58" s="8"/>
       <c r="Q58" s="8"/>
-      <c r="R58" s="23"/>
+      <c r="R58" s="26"/>
       <c r="S58" s="6"/>
-      <c r="T58" s="28"/>
+      <c r="T58" s="31"/>
       <c r="W58" s="20">
         <v>5</v>
       </c>
@@ -6080,9 +6110,9 @@
       <c r="O59" s="8"/>
       <c r="P59" s="8"/>
       <c r="Q59" s="8"/>
-      <c r="R59" s="23"/>
+      <c r="R59" s="26"/>
       <c r="S59" s="6"/>
-      <c r="T59" s="28"/>
+      <c r="T59" s="31"/>
       <c r="W59" s="20">
         <v>6</v>
       </c>
@@ -6110,9 +6140,9 @@
       <c r="O60" s="8"/>
       <c r="P60" s="8"/>
       <c r="Q60" s="8"/>
-      <c r="R60" s="23"/>
+      <c r="R60" s="26"/>
       <c r="S60" s="6"/>
-      <c r="T60" s="28"/>
+      <c r="T60" s="31"/>
       <c r="W60" s="20">
         <v>7</v>
       </c>
@@ -6140,11 +6170,11 @@
       <c r="O61" s="8"/>
       <c r="P61" s="8"/>
       <c r="Q61" s="8"/>
-      <c r="R61" s="23"/>
+      <c r="R61" s="26"/>
       <c r="S61" t="s">
         <v>17</v>
       </c>
-      <c r="T61" s="28"/>
+      <c r="T61" s="31"/>
       <c r="W61" s="20">
         <v>8</v>
       </c>
@@ -6172,11 +6202,11 @@
       <c r="O62" s="17"/>
       <c r="P62" s="17"/>
       <c r="Q62" s="17"/>
-      <c r="R62" s="23"/>
+      <c r="R62" s="26"/>
       <c r="S62" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T62" s="28"/>
+      <c r="T62" s="31"/>
       <c r="W62" s="20">
         <v>9</v>
       </c>
@@ -6210,7 +6240,7 @@
       <c r="S63" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T63" s="28"/>
+      <c r="T63" s="31"/>
       <c r="W63" s="20">
         <v>10</v>
       </c>
@@ -6244,7 +6274,7 @@
       <c r="S64" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T64" s="28"/>
+      <c r="T64" s="31"/>
       <c r="W64" s="20">
         <v>11</v>
       </c>
@@ -6278,7 +6308,7 @@
       <c r="S65" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T65" s="28"/>
+      <c r="T65" s="31"/>
       <c r="U65" t="s">
         <v>28</v>
       </c>
@@ -6315,7 +6345,7 @@
       <c r="S66" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T66" s="28"/>
+      <c r="T66" s="31"/>
       <c r="U66" t="s">
         <v>30</v>
       </c>
@@ -6346,7 +6376,7 @@
       <c r="S67" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T67" s="28"/>
+      <c r="T67" s="31"/>
       <c r="U67" t="s">
         <v>32</v>
       </c>
@@ -6377,7 +6407,7 @@
       <c r="S68" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T68" s="28"/>
+      <c r="T68" s="31"/>
       <c r="U68" t="s">
         <v>34</v>
       </c>
@@ -6458,11 +6488,11 @@
       <c r="O72" s="8"/>
       <c r="P72" s="8"/>
       <c r="Q72" s="8"/>
-      <c r="R72" s="23" t="s">
+      <c r="R72" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S72" s="6"/>
-      <c r="T72" s="29" t="s">
+      <c r="T72" s="32" t="s">
         <v>94</v>
       </c>
     </row>
@@ -6486,9 +6516,9 @@
       <c r="O73" s="8"/>
       <c r="P73" s="8"/>
       <c r="Q73" s="8"/>
-      <c r="R73" s="23"/>
+      <c r="R73" s="26"/>
       <c r="S73" s="6"/>
-      <c r="T73" s="30"/>
+      <c r="T73" s="33"/>
     </row>
     <row r="74" spans="1:24" ht="18.75" customHeight="1">
       <c r="A74" s="6" t="s">
@@ -6510,9 +6540,9 @@
       <c r="O74" s="8"/>
       <c r="P74" s="8"/>
       <c r="Q74" s="8"/>
-      <c r="R74" s="23"/>
+      <c r="R74" s="26"/>
       <c r="S74" s="6"/>
-      <c r="T74" s="30"/>
+      <c r="T74" s="33"/>
     </row>
     <row r="75" spans="1:24" ht="18.75" customHeight="1">
       <c r="A75" s="6" t="s">
@@ -6534,9 +6564,9 @@
       <c r="O75" s="8"/>
       <c r="P75" s="8"/>
       <c r="Q75" s="8"/>
-      <c r="R75" s="23"/>
+      <c r="R75" s="26"/>
       <c r="S75" s="6"/>
-      <c r="T75" s="30"/>
+      <c r="T75" s="33"/>
     </row>
     <row r="76" spans="1:24" ht="15.75" customHeight="1">
       <c r="A76" s="6" t="s">
@@ -6558,9 +6588,9 @@
       <c r="O76" s="8"/>
       <c r="P76" s="8"/>
       <c r="Q76" s="8"/>
-      <c r="R76" s="23"/>
+      <c r="R76" s="26"/>
       <c r="S76" s="6"/>
-      <c r="T76" s="30"/>
+      <c r="T76" s="33"/>
     </row>
     <row r="77" spans="1:24" ht="15.75" customHeight="1">
       <c r="A77" s="6" t="s">
@@ -6582,9 +6612,9 @@
       <c r="O77" s="8"/>
       <c r="P77" s="8"/>
       <c r="Q77" s="8"/>
-      <c r="R77" s="23"/>
+      <c r="R77" s="26"/>
       <c r="S77" s="6"/>
-      <c r="T77" s="30"/>
+      <c r="T77" s="33"/>
     </row>
     <row r="78" spans="1:24" ht="15.75" customHeight="1">
       <c r="A78" s="6" t="s">
@@ -6606,9 +6636,9 @@
       <c r="O78" s="8"/>
       <c r="P78" s="8"/>
       <c r="Q78" s="8"/>
-      <c r="R78" s="23"/>
+      <c r="R78" s="26"/>
       <c r="S78" s="6"/>
-      <c r="T78" s="30"/>
+      <c r="T78" s="33"/>
     </row>
     <row r="79" spans="1:24" ht="15" customHeight="1">
       <c r="A79" s="6" t="s">
@@ -6630,11 +6660,11 @@
       <c r="O79" s="17"/>
       <c r="P79" s="17"/>
       <c r="Q79" s="17"/>
-      <c r="R79" s="23"/>
+      <c r="R79" s="26"/>
       <c r="S79" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T79" s="30"/>
+      <c r="T79" s="33"/>
     </row>
     <row r="80" spans="1:24" ht="15" customHeight="1">
       <c r="A80" s="6" t="s">
@@ -6662,7 +6692,7 @@
       <c r="S80" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T80" s="30"/>
+      <c r="T80" s="33"/>
     </row>
     <row r="81" spans="1:21" ht="15" customHeight="1">
       <c r="A81" s="6" t="s">
@@ -6690,7 +6720,7 @@
       <c r="S81" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T81" s="30"/>
+      <c r="T81" s="33"/>
     </row>
     <row r="82" spans="1:21" ht="15" customHeight="1">
       <c r="A82" s="6" t="s">
@@ -6718,7 +6748,7 @@
       <c r="S82" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T82" s="30"/>
+      <c r="T82" s="33"/>
       <c r="U82" t="s">
         <v>28</v>
       </c>
@@ -6749,7 +6779,7 @@
       <c r="S83" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T83" s="30"/>
+      <c r="T83" s="33"/>
       <c r="U83" t="s">
         <v>30</v>
       </c>
@@ -6780,7 +6810,7 @@
       <c r="S84" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T84" s="30"/>
+      <c r="T84" s="33"/>
       <c r="U84" t="s">
         <v>32</v>
       </c>
@@ -6811,7 +6841,7 @@
       <c r="S85" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T85" s="31"/>
+      <c r="T85" s="34"/>
       <c r="U85" t="s">
         <v>34</v>
       </c>
@@ -6892,11 +6922,11 @@
       <c r="O89" s="8"/>
       <c r="P89" s="8"/>
       <c r="Q89" s="8"/>
-      <c r="R89" s="23" t="s">
+      <c r="R89" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S89" s="6"/>
-      <c r="T89" s="28" t="s">
+      <c r="T89" s="31" t="s">
         <v>109</v>
       </c>
     </row>
@@ -6920,9 +6950,9 @@
       <c r="O90" s="8"/>
       <c r="P90" s="8"/>
       <c r="Q90" s="8"/>
-      <c r="R90" s="23"/>
+      <c r="R90" s="26"/>
       <c r="S90" s="6"/>
-      <c r="T90" s="28"/>
+      <c r="T90" s="31"/>
     </row>
     <row r="91" spans="1:21" ht="15.75">
       <c r="A91" s="6" t="s">
@@ -6944,9 +6974,9 @@
       <c r="O91" s="8"/>
       <c r="P91" s="8"/>
       <c r="Q91" s="8"/>
-      <c r="R91" s="23"/>
+      <c r="R91" s="26"/>
       <c r="S91" s="6"/>
-      <c r="T91" s="28"/>
+      <c r="T91" s="31"/>
     </row>
     <row r="92" spans="1:21" ht="15.75">
       <c r="A92" s="6" t="s">
@@ -6968,9 +6998,9 @@
       <c r="O92" s="8"/>
       <c r="P92" s="8"/>
       <c r="Q92" s="8"/>
-      <c r="R92" s="23"/>
+      <c r="R92" s="26"/>
       <c r="S92" s="6"/>
-      <c r="T92" s="28"/>
+      <c r="T92" s="31"/>
     </row>
     <row r="93" spans="1:21" ht="15.75">
       <c r="A93" s="6" t="s">
@@ -6992,9 +7022,9 @@
       <c r="O93" s="8"/>
       <c r="P93" s="8"/>
       <c r="Q93" s="8"/>
-      <c r="R93" s="23"/>
+      <c r="R93" s="26"/>
       <c r="S93" s="6"/>
-      <c r="T93" s="28"/>
+      <c r="T93" s="31"/>
     </row>
     <row r="94" spans="1:21" ht="15.75">
       <c r="A94" s="6" t="s">
@@ -7016,9 +7046,9 @@
       <c r="O94" s="8"/>
       <c r="P94" s="8"/>
       <c r="Q94" s="8"/>
-      <c r="R94" s="23"/>
+      <c r="R94" s="26"/>
       <c r="S94" s="6"/>
-      <c r="T94" s="28"/>
+      <c r="T94" s="31"/>
     </row>
     <row r="95" spans="1:21" ht="15.75">
       <c r="A95" s="6" t="s">
@@ -7040,9 +7070,9 @@
       <c r="O95" s="8"/>
       <c r="P95" s="8"/>
       <c r="Q95" s="8"/>
-      <c r="R95" s="23"/>
+      <c r="R95" s="26"/>
       <c r="S95" s="6"/>
-      <c r="T95" s="28"/>
+      <c r="T95" s="31"/>
     </row>
     <row r="96" spans="1:21">
       <c r="A96" s="6" t="s">
@@ -7064,11 +7094,11 @@
       <c r="O96" s="17"/>
       <c r="P96" s="17"/>
       <c r="Q96" s="17"/>
-      <c r="R96" s="23"/>
+      <c r="R96" s="26"/>
       <c r="S96" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T96" s="28"/>
+      <c r="T96" s="31"/>
     </row>
     <row r="97" spans="1:21" ht="15" customHeight="1">
       <c r="A97" s="6" t="s">
@@ -7096,7 +7126,7 @@
       <c r="S97" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T97" s="28"/>
+      <c r="T97" s="31"/>
     </row>
     <row r="98" spans="1:21" ht="15" customHeight="1">
       <c r="A98" s="6" t="s">
@@ -7124,7 +7154,7 @@
       <c r="S98" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T98" s="28"/>
+      <c r="T98" s="31"/>
     </row>
     <row r="99" spans="1:21" ht="15" customHeight="1">
       <c r="A99" s="6" t="s">
@@ -7152,7 +7182,7 @@
       <c r="S99" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T99" s="28"/>
+      <c r="T99" s="31"/>
       <c r="U99" t="s">
         <v>28</v>
       </c>
@@ -7183,7 +7213,7 @@
       <c r="S100" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T100" s="28"/>
+      <c r="T100" s="31"/>
       <c r="U100" t="s">
         <v>30</v>
       </c>
@@ -7214,7 +7244,7 @@
       <c r="S101" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T101" s="28"/>
+      <c r="T101" s="31"/>
       <c r="U101" t="s">
         <v>32</v>
       </c>
@@ -7245,7 +7275,7 @@
       <c r="S102" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T102" s="28"/>
+      <c r="T102" s="31"/>
       <c r="U102" t="s">
         <v>34</v>
       </c>
@@ -7326,11 +7356,11 @@
       <c r="O106" s="8"/>
       <c r="P106" s="8"/>
       <c r="Q106" s="8"/>
-      <c r="R106" s="23" t="s">
+      <c r="R106" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S106" s="22"/>
-      <c r="T106" s="24" t="s">
+      <c r="T106" s="27" t="s">
         <v>124</v>
       </c>
     </row>
@@ -7354,9 +7384,9 @@
       <c r="O107" s="8"/>
       <c r="P107" s="8"/>
       <c r="Q107" s="8"/>
-      <c r="R107" s="23"/>
+      <c r="R107" s="26"/>
       <c r="S107" s="22"/>
-      <c r="T107" s="24"/>
+      <c r="T107" s="27"/>
     </row>
     <row r="108" spans="1:21" ht="15.75">
       <c r="A108" s="6" t="s">
@@ -7378,9 +7408,9 @@
       <c r="O108" s="8"/>
       <c r="P108" s="8"/>
       <c r="Q108" s="8"/>
-      <c r="R108" s="23"/>
+      <c r="R108" s="26"/>
       <c r="S108" s="22"/>
-      <c r="T108" s="24"/>
+      <c r="T108" s="27"/>
     </row>
     <row r="109" spans="1:21" ht="15.75">
       <c r="A109" s="6" t="s">
@@ -7402,9 +7432,9 @@
       <c r="O109" s="8"/>
       <c r="P109" s="8"/>
       <c r="Q109" s="8"/>
-      <c r="R109" s="23"/>
+      <c r="R109" s="26"/>
       <c r="S109" s="22"/>
-      <c r="T109" s="24"/>
+      <c r="T109" s="27"/>
     </row>
     <row r="110" spans="1:21" ht="15.75">
       <c r="A110" s="6" t="s">
@@ -7426,9 +7456,9 @@
       <c r="O110" s="8"/>
       <c r="P110" s="8"/>
       <c r="Q110" s="8"/>
-      <c r="R110" s="23"/>
+      <c r="R110" s="26"/>
       <c r="S110" s="22"/>
-      <c r="T110" s="24"/>
+      <c r="T110" s="27"/>
     </row>
     <row r="111" spans="1:21" ht="15.75">
       <c r="A111" s="6" t="s">
@@ -7450,9 +7480,9 @@
       <c r="O111" s="8"/>
       <c r="P111" s="8"/>
       <c r="Q111" s="8"/>
-      <c r="R111" s="23"/>
+      <c r="R111" s="26"/>
       <c r="S111" s="22"/>
-      <c r="T111" s="24"/>
+      <c r="T111" s="27"/>
     </row>
     <row r="112" spans="1:21" ht="15.75">
       <c r="A112" s="6" t="s">
@@ -7474,9 +7504,9 @@
       <c r="O112" s="8"/>
       <c r="P112" s="8"/>
       <c r="Q112" s="8"/>
-      <c r="R112" s="23"/>
+      <c r="R112" s="26"/>
       <c r="S112" s="22"/>
-      <c r="T112" s="24"/>
+      <c r="T112" s="27"/>
     </row>
     <row r="113" spans="1:21">
       <c r="A113" s="6" t="s">
@@ -7498,11 +7528,11 @@
       <c r="O113" s="17"/>
       <c r="P113" s="17"/>
       <c r="Q113" s="17"/>
-      <c r="R113" s="23"/>
+      <c r="R113" s="26"/>
       <c r="S113" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T113" s="24"/>
+      <c r="T113" s="27"/>
     </row>
     <row r="114" spans="1:21" ht="15" customHeight="1">
       <c r="A114" s="6" t="s">
@@ -7530,7 +7560,7 @@
       <c r="S114" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T114" s="24"/>
+      <c r="T114" s="27"/>
     </row>
     <row r="115" spans="1:21" ht="15" customHeight="1">
       <c r="A115" s="6" t="s">
@@ -7558,7 +7588,7 @@
       <c r="S115" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T115" s="24"/>
+      <c r="T115" s="27"/>
     </row>
     <row r="116" spans="1:21" ht="15" customHeight="1">
       <c r="A116" s="6" t="s">
@@ -7586,7 +7616,7 @@
       <c r="S116" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T116" s="24"/>
+      <c r="T116" s="27"/>
       <c r="U116" t="s">
         <v>28</v>
       </c>
@@ -7617,7 +7647,7 @@
       <c r="S117" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T117" s="24"/>
+      <c r="T117" s="27"/>
       <c r="U117" t="s">
         <v>30</v>
       </c>
@@ -7648,7 +7678,7 @@
       <c r="S118" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T118" s="24"/>
+      <c r="T118" s="27"/>
       <c r="U118" t="s">
         <v>32</v>
       </c>
@@ -7679,7 +7709,7 @@
       <c r="S119" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T119" s="24"/>
+      <c r="T119" s="27"/>
       <c r="U119" t="s">
         <v>34</v>
       </c>
@@ -7760,11 +7790,11 @@
       <c r="O123" s="8"/>
       <c r="P123" s="8"/>
       <c r="Q123" s="8"/>
-      <c r="R123" s="23" t="s">
+      <c r="R123" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S123" s="22"/>
-      <c r="T123" s="24" t="s">
+      <c r="T123" s="27" t="s">
         <v>139</v>
       </c>
     </row>
@@ -7788,9 +7818,9 @@
       <c r="O124" s="8"/>
       <c r="P124" s="8"/>
       <c r="Q124" s="8"/>
-      <c r="R124" s="23"/>
+      <c r="R124" s="26"/>
       <c r="S124" s="22"/>
-      <c r="T124" s="24"/>
+      <c r="T124" s="27"/>
     </row>
     <row r="125" spans="1:21" ht="15.75">
       <c r="A125" s="6" t="s">
@@ -7812,9 +7842,9 @@
       <c r="O125" s="8"/>
       <c r="P125" s="8"/>
       <c r="Q125" s="8"/>
-      <c r="R125" s="23"/>
+      <c r="R125" s="26"/>
       <c r="S125" s="22"/>
-      <c r="T125" s="24"/>
+      <c r="T125" s="27"/>
     </row>
     <row r="126" spans="1:21" ht="15.75">
       <c r="A126" s="6" t="s">
@@ -7836,9 +7866,9 @@
       <c r="O126" s="8"/>
       <c r="P126" s="8"/>
       <c r="Q126" s="8"/>
-      <c r="R126" s="23"/>
+      <c r="R126" s="26"/>
       <c r="S126" s="22"/>
-      <c r="T126" s="24"/>
+      <c r="T126" s="27"/>
     </row>
     <row r="127" spans="1:21" ht="15.75">
       <c r="A127" s="6" t="s">
@@ -7860,9 +7890,9 @@
       <c r="O127" s="8"/>
       <c r="P127" s="8"/>
       <c r="Q127" s="8"/>
-      <c r="R127" s="23"/>
+      <c r="R127" s="26"/>
       <c r="S127" s="22"/>
-      <c r="T127" s="24"/>
+      <c r="T127" s="27"/>
     </row>
     <row r="128" spans="1:21" ht="15.75">
       <c r="A128" s="6" t="s">
@@ -7884,9 +7914,9 @@
       <c r="O128" s="8"/>
       <c r="P128" s="8"/>
       <c r="Q128" s="8"/>
-      <c r="R128" s="23"/>
+      <c r="R128" s="26"/>
       <c r="S128" s="22"/>
-      <c r="T128" s="24"/>
+      <c r="T128" s="27"/>
     </row>
     <row r="129" spans="1:21" ht="15.75" customHeight="1">
       <c r="A129" s="6" t="s">
@@ -7908,9 +7938,9 @@
       <c r="O129" s="8"/>
       <c r="P129" s="8"/>
       <c r="Q129" s="8"/>
-      <c r="R129" s="23"/>
+      <c r="R129" s="26"/>
       <c r="S129" s="22"/>
-      <c r="T129" s="24"/>
+      <c r="T129" s="27"/>
     </row>
     <row r="130" spans="1:21" ht="15" customHeight="1">
       <c r="A130" s="6" t="s">
@@ -7932,11 +7962,11 @@
       <c r="O130" s="17"/>
       <c r="P130" s="17"/>
       <c r="Q130" s="17"/>
-      <c r="R130" s="23"/>
+      <c r="R130" s="26"/>
       <c r="S130" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T130" s="24"/>
+      <c r="T130" s="27"/>
     </row>
     <row r="131" spans="1:21" ht="15" customHeight="1">
       <c r="A131" s="6" t="s">
@@ -7964,7 +7994,7 @@
       <c r="S131" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T131" s="24"/>
+      <c r="T131" s="27"/>
     </row>
     <row r="132" spans="1:21" ht="15" customHeight="1">
       <c r="A132" s="6" t="s">
@@ -7992,7 +8022,7 @@
       <c r="S132" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T132" s="24"/>
+      <c r="T132" s="27"/>
     </row>
     <row r="133" spans="1:21" ht="15" customHeight="1">
       <c r="A133" s="6" t="s">
@@ -8020,7 +8050,7 @@
       <c r="S133" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T133" s="24"/>
+      <c r="T133" s="27"/>
       <c r="U133" t="s">
         <v>28</v>
       </c>
@@ -8051,7 +8081,7 @@
       <c r="S134" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T134" s="24"/>
+      <c r="T134" s="27"/>
       <c r="U134" t="s">
         <v>30</v>
       </c>
@@ -8082,7 +8112,7 @@
       <c r="S135" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T135" s="24"/>
+      <c r="T135" s="27"/>
       <c r="U135" t="s">
         <v>32</v>
       </c>
@@ -8175,11 +8205,11 @@
       <c r="O140" s="8"/>
       <c r="P140" s="8"/>
       <c r="Q140" s="8"/>
-      <c r="R140" s="23" t="s">
+      <c r="R140" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S140" s="22"/>
-      <c r="T140" s="25" t="s">
+      <c r="T140" s="28" t="s">
         <v>153</v>
       </c>
     </row>
@@ -8203,9 +8233,9 @@
       <c r="O141" s="8"/>
       <c r="P141" s="8"/>
       <c r="Q141" s="8"/>
-      <c r="R141" s="23"/>
+      <c r="R141" s="26"/>
       <c r="S141" s="22"/>
-      <c r="T141" s="26"/>
+      <c r="T141" s="29"/>
     </row>
     <row r="142" spans="1:21" ht="15.75">
       <c r="A142" s="6" t="s">
@@ -8227,9 +8257,9 @@
       <c r="O142" s="8"/>
       <c r="P142" s="8"/>
       <c r="Q142" s="8"/>
-      <c r="R142" s="23"/>
+      <c r="R142" s="26"/>
       <c r="S142" s="22"/>
-      <c r="T142" s="26"/>
+      <c r="T142" s="29"/>
     </row>
     <row r="143" spans="1:21" ht="15.75">
       <c r="A143" s="6" t="s">
@@ -8251,9 +8281,9 @@
       <c r="O143" s="8"/>
       <c r="P143" s="8"/>
       <c r="Q143" s="8"/>
-      <c r="R143" s="23"/>
+      <c r="R143" s="26"/>
       <c r="S143" s="22"/>
-      <c r="T143" s="26"/>
+      <c r="T143" s="29"/>
     </row>
     <row r="144" spans="1:21" ht="15.75">
       <c r="A144" s="6" t="s">
@@ -8275,9 +8305,9 @@
       <c r="O144" s="8"/>
       <c r="P144" s="8"/>
       <c r="Q144" s="8"/>
-      <c r="R144" s="23"/>
+      <c r="R144" s="26"/>
       <c r="S144" s="22"/>
-      <c r="T144" s="26"/>
+      <c r="T144" s="29"/>
     </row>
     <row r="145" spans="1:22" ht="15.75">
       <c r="A145" s="6" t="s">
@@ -8299,9 +8329,9 @@
       <c r="O145" s="8"/>
       <c r="P145" s="8"/>
       <c r="Q145" s="8"/>
-      <c r="R145" s="23"/>
+      <c r="R145" s="26"/>
       <c r="S145" s="22"/>
-      <c r="T145" s="26"/>
+      <c r="T145" s="29"/>
     </row>
     <row r="146" spans="1:22" ht="15.75">
       <c r="A146" s="6" t="s">
@@ -8323,9 +8353,9 @@
       <c r="O146" s="8"/>
       <c r="P146" s="8"/>
       <c r="Q146" s="8"/>
-      <c r="R146" s="23"/>
+      <c r="R146" s="26"/>
       <c r="S146" s="22"/>
-      <c r="T146" s="26"/>
+      <c r="T146" s="29"/>
     </row>
     <row r="147" spans="1:22">
       <c r="A147" s="6" t="s">
@@ -8347,11 +8377,11 @@
       <c r="O147" s="17"/>
       <c r="P147" s="17"/>
       <c r="Q147" s="17"/>
-      <c r="R147" s="23"/>
+      <c r="R147" s="26"/>
       <c r="S147" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T147" s="26"/>
+      <c r="T147" s="29"/>
     </row>
     <row r="148" spans="1:22">
       <c r="A148" s="6" t="s">
@@ -8379,7 +8409,7 @@
       <c r="S148" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T148" s="26"/>
+      <c r="T148" s="29"/>
     </row>
     <row r="149" spans="1:22">
       <c r="A149" s="6" t="s">
@@ -8407,7 +8437,7 @@
       <c r="S149" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T149" s="26"/>
+      <c r="T149" s="29"/>
     </row>
     <row r="150" spans="1:22">
       <c r="A150" s="6"/>
@@ -8428,7 +8458,7 @@
       <c r="P150" s="6"/>
       <c r="Q150" s="6"/>
       <c r="R150" s="6"/>
-      <c r="T150" s="26"/>
+      <c r="T150" s="29"/>
     </row>
     <row r="151" spans="1:22">
       <c r="A151" s="6" t="s">
@@ -8456,7 +8486,7 @@
       <c r="S151" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T151" s="26"/>
+      <c r="T151" s="29"/>
       <c r="U151" t="s">
         <v>28</v>
       </c>
@@ -8487,7 +8517,7 @@
       <c r="S152" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T152" s="26"/>
+      <c r="T152" s="29"/>
       <c r="U152" t="s">
         <v>30</v>
       </c>
@@ -8518,7 +8548,7 @@
       <c r="S153" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T153" s="27"/>
+      <c r="T153" s="30"/>
       <c r="U153" t="s">
         <v>32</v>
       </c>
@@ -8629,17 +8659,17 @@
       <c r="O158" s="8"/>
       <c r="P158" s="8"/>
       <c r="Q158" s="8"/>
-      <c r="R158" s="23" t="s">
+      <c r="R158" s="26" t="s">
         <v>9</v>
       </c>
       <c r="S158" s="22"/>
-      <c r="T158" s="24" t="s">
+      <c r="T158" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="U158" s="36" t="s">
+      <c r="U158" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="V158" s="34"/>
+      <c r="V158" s="38"/>
     </row>
     <row r="159" spans="1:22" ht="15.75" customHeight="1">
       <c r="A159" s="6" t="s">
@@ -8661,9 +8691,9 @@
       <c r="O159" s="8"/>
       <c r="P159" s="8"/>
       <c r="Q159" s="8"/>
-      <c r="R159" s="23"/>
+      <c r="R159" s="26"/>
       <c r="S159" s="22"/>
-      <c r="T159" s="24"/>
+      <c r="T159" s="27"/>
     </row>
     <row r="160" spans="1:22" ht="15.75" customHeight="1">
       <c r="A160" s="6" t="s">
@@ -8685,9 +8715,9 @@
       <c r="O160" s="8"/>
       <c r="P160" s="8"/>
       <c r="Q160" s="8"/>
-      <c r="R160" s="23"/>
+      <c r="R160" s="26"/>
       <c r="S160" s="22"/>
-      <c r="T160" s="24"/>
+      <c r="T160" s="27"/>
     </row>
     <row r="161" spans="1:22" ht="15.75" customHeight="1">
       <c r="A161" s="6" t="s">
@@ -8709,9 +8739,9 @@
       <c r="O161" s="8"/>
       <c r="P161" s="8"/>
       <c r="Q161" s="8"/>
-      <c r="R161" s="23"/>
+      <c r="R161" s="26"/>
       <c r="S161" s="22"/>
-      <c r="T161" s="24"/>
+      <c r="T161" s="27"/>
     </row>
     <row r="162" spans="1:22" ht="15.75" customHeight="1">
       <c r="A162" s="6" t="s">
@@ -8733,9 +8763,9 @@
       <c r="O162" s="8"/>
       <c r="P162" s="8"/>
       <c r="Q162" s="8"/>
-      <c r="R162" s="23"/>
+      <c r="R162" s="26"/>
       <c r="S162" s="22"/>
-      <c r="T162" s="24"/>
+      <c r="T162" s="27"/>
     </row>
     <row r="163" spans="1:22" ht="15.75" customHeight="1">
       <c r="A163" s="6" t="s">
@@ -8757,9 +8787,9 @@
       <c r="O163" s="8"/>
       <c r="P163" s="8"/>
       <c r="Q163" s="8"/>
-      <c r="R163" s="23"/>
+      <c r="R163" s="26"/>
       <c r="S163" s="22"/>
-      <c r="T163" s="24"/>
+      <c r="T163" s="27"/>
     </row>
     <row r="164" spans="1:22" ht="15.75" customHeight="1">
       <c r="A164" s="6" t="s">
@@ -8781,9 +8811,9 @@
       <c r="O164" s="8"/>
       <c r="P164" s="8"/>
       <c r="Q164" s="8"/>
-      <c r="R164" s="23"/>
+      <c r="R164" s="26"/>
       <c r="S164" s="22"/>
-      <c r="T164" s="24"/>
+      <c r="T164" s="27"/>
     </row>
     <row r="165" spans="1:22" ht="15" customHeight="1">
       <c r="A165" s="6" t="s">
@@ -8805,11 +8835,11 @@
       <c r="O165" s="17"/>
       <c r="P165" s="17"/>
       <c r="Q165" s="17"/>
-      <c r="R165" s="23"/>
-      <c r="S165" s="35" t="s">
+      <c r="R165" s="26"/>
+      <c r="S165" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="T165" s="24"/>
+      <c r="T165" s="27"/>
     </row>
     <row r="166" spans="1:22" ht="15" customHeight="1">
       <c r="A166" s="6" t="s">
@@ -8837,7 +8867,7 @@
       <c r="S166" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T166" s="24"/>
+      <c r="T166" s="27"/>
     </row>
     <row r="167" spans="1:22" ht="15" customHeight="1">
       <c r="A167" s="6" t="s">
@@ -8865,42 +8895,37 @@
       <c r="S167" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T167" s="24"/>
+      <c r="T167" s="27"/>
     </row>
     <row r="168" spans="1:22" ht="15" customHeight="1">
       <c r="A168" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B168" s="6"/>
-      <c r="C168" s="6"/>
-      <c r="D168" s="6"/>
-      <c r="E168" s="6"/>
-      <c r="F168" s="6"/>
-      <c r="G168" s="6"/>
-      <c r="H168" s="6"/>
-      <c r="I168" s="6"/>
-      <c r="J168" s="6"/>
-      <c r="K168" s="6"/>
-      <c r="L168" s="6"/>
-      <c r="M168" s="6"/>
-      <c r="N168" s="6"/>
-      <c r="O168" s="6"/>
-      <c r="P168" s="6"/>
-      <c r="Q168" s="16"/>
-      <c r="R168" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S168" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="T168" s="24"/>
-      <c r="U168" t="s">
-        <v>28</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="B168" s="12"/>
+      <c r="C168" s="12"/>
+      <c r="D168" s="12"/>
+      <c r="E168" s="12"/>
+      <c r="F168" s="12"/>
+      <c r="G168" s="12"/>
+      <c r="H168" s="12"/>
+      <c r="I168" s="12"/>
+      <c r="J168" s="12"/>
+      <c r="K168" s="12"/>
+      <c r="L168" s="12"/>
+      <c r="M168" s="12"/>
+      <c r="N168" s="12"/>
+      <c r="O168" s="12"/>
+      <c r="P168" s="12"/>
+      <c r="Q168" s="12"/>
+      <c r="R168" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="S168" s="22"/>
+      <c r="T168" s="27"/>
     </row>
     <row r="169" spans="1:22" ht="15" customHeight="1">
       <c r="A169" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
@@ -8924,14 +8949,14 @@
       <c r="S169" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T169" s="24"/>
+      <c r="T169" s="27"/>
       <c r="U169" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="170" spans="1:22" ht="15" customHeight="1">
       <c r="A170" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
@@ -8955,12 +8980,30 @@
       <c r="S170" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T170" s="24"/>
+      <c r="T170" s="27"/>
       <c r="U170" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="171" spans="1:22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="171" spans="1:22" ht="15" customHeight="1">
+      <c r="A171" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B171" s="6"/>
+      <c r="C171" s="6"/>
+      <c r="D171" s="6"/>
+      <c r="E171" s="6"/>
+      <c r="F171" s="6"/>
+      <c r="G171" s="6"/>
+      <c r="H171" s="6"/>
+      <c r="I171" s="6"/>
+      <c r="J171" s="6"/>
+      <c r="K171" s="6"/>
+      <c r="L171" s="6"/>
+      <c r="M171" s="6"/>
+      <c r="N171" s="6"/>
+      <c r="O171" s="6"/>
+      <c r="P171" s="6"/>
       <c r="Q171" s="16"/>
       <c r="R171" s="6" t="s">
         <v>27</v>
@@ -8968,102 +9011,83 @@
       <c r="S171" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T171" s="24"/>
+      <c r="T171" s="27"/>
       <c r="U171" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="172" spans="1:22">
+      <c r="Q172" s="16"/>
+      <c r="R172" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S172" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="T172" s="27"/>
+      <c r="U172" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="174" spans="1:22" ht="15.75">
-      <c r="A174" s="3" t="s">
+    <row r="175" spans="1:22" ht="15.75">
+      <c r="A175" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B174" s="1" t="s">
+      <c r="B175" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C174" s="1" t="s">
+      <c r="C175" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D174" s="1" t="s">
+      <c r="D175" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E174" s="1" t="s">
+      <c r="E175" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F174" s="1" t="s">
+      <c r="F175" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G174" s="1" t="s">
+      <c r="G175" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H174" s="1">
+      <c r="H175" s="1">
         <v>9</v>
       </c>
-      <c r="I174" s="2">
+      <c r="I175" s="2">
         <v>8</v>
       </c>
-      <c r="J174" s="2">
+      <c r="J175" s="2">
         <v>7</v>
       </c>
-      <c r="K174" s="2">
+      <c r="K175" s="2">
         <v>6</v>
       </c>
-      <c r="L174" s="2">
+      <c r="L175" s="2">
         <v>5</v>
       </c>
-      <c r="M174" s="2">
+      <c r="M175" s="2">
         <v>4</v>
       </c>
-      <c r="N174" s="2">
+      <c r="N175" s="2">
         <v>3</v>
       </c>
-      <c r="O174" s="2">
+      <c r="O175" s="2">
         <v>2</v>
       </c>
-      <c r="P174" s="2">
+      <c r="P175" s="2">
         <v>1</v>
       </c>
-      <c r="Q174" s="2">
+      <c r="Q175" s="2">
         <v>0</v>
       </c>
-      <c r="R174" t="s">
+      <c r="R175" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="175" spans="1:22" ht="15.75">
-      <c r="A175" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="B175" s="7"/>
-      <c r="C175" s="7"/>
-      <c r="D175" s="7"/>
-      <c r="E175" s="7"/>
-      <c r="F175" s="7"/>
-      <c r="G175" s="7"/>
-      <c r="H175" s="7"/>
-      <c r="I175" s="8"/>
-      <c r="J175" s="8"/>
-      <c r="K175" s="8"/>
-      <c r="L175" s="8"/>
-      <c r="M175" s="8"/>
-      <c r="N175" s="8"/>
-      <c r="O175" s="8"/>
-      <c r="P175" s="8"/>
-      <c r="Q175" s="8"/>
-      <c r="R175" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="S175" s="22"/>
-      <c r="T175" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="U175" s="36" t="s">
-        <v>170</v>
-      </c>
-      <c r="V175" s="34"/>
     </row>
     <row r="176" spans="1:22" ht="15.75">
       <c r="A176" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
@@ -9081,13 +9105,21 @@
       <c r="O176" s="8"/>
       <c r="P176" s="8"/>
       <c r="Q176" s="8"/>
-      <c r="R176" s="23"/>
+      <c r="R176" s="26" t="s">
+        <v>9</v>
+      </c>
       <c r="S176" s="22"/>
-      <c r="T176" s="24"/>
+      <c r="T176" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="U176" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="V176" s="38"/>
     </row>
     <row r="177" spans="1:20" ht="15.75">
       <c r="A177" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
@@ -9105,13 +9137,13 @@
       <c r="O177" s="8"/>
       <c r="P177" s="8"/>
       <c r="Q177" s="8"/>
-      <c r="R177" s="23"/>
+      <c r="R177" s="26"/>
       <c r="S177" s="22"/>
-      <c r="T177" s="24"/>
+      <c r="T177" s="27"/>
     </row>
     <row r="178" spans="1:20" ht="15.75">
       <c r="A178" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
@@ -9129,13 +9161,13 @@
       <c r="O178" s="8"/>
       <c r="P178" s="8"/>
       <c r="Q178" s="8"/>
-      <c r="R178" s="23"/>
+      <c r="R178" s="26"/>
       <c r="S178" s="22"/>
-      <c r="T178" s="24"/>
+      <c r="T178" s="27"/>
     </row>
     <row r="179" spans="1:20" ht="15.75">
       <c r="A179" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
@@ -9153,13 +9185,13 @@
       <c r="O179" s="8"/>
       <c r="P179" s="8"/>
       <c r="Q179" s="8"/>
-      <c r="R179" s="23"/>
+      <c r="R179" s="26"/>
       <c r="S179" s="22"/>
-      <c r="T179" s="24"/>
+      <c r="T179" s="27"/>
     </row>
     <row r="180" spans="1:20" ht="15.75">
       <c r="A180" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
@@ -9177,13 +9209,13 @@
       <c r="O180" s="8"/>
       <c r="P180" s="8"/>
       <c r="Q180" s="8"/>
-      <c r="R180" s="23"/>
+      <c r="R180" s="26"/>
       <c r="S180" s="22"/>
-      <c r="T180" s="24"/>
+      <c r="T180" s="27"/>
     </row>
     <row r="181" spans="1:20" ht="15.75">
       <c r="A181" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
@@ -9201,65 +9233,63 @@
       <c r="O181" s="8"/>
       <c r="P181" s="8"/>
       <c r="Q181" s="8"/>
-      <c r="R181" s="23"/>
+      <c r="R181" s="26"/>
       <c r="S181" s="22"/>
-      <c r="T181" s="24"/>
-    </row>
-    <row r="182" spans="1:20">
+      <c r="T181" s="27"/>
+    </row>
+    <row r="182" spans="1:20" ht="15.75">
       <c r="A182" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B182" s="17"/>
-      <c r="C182" s="17"/>
-      <c r="D182" s="17"/>
-      <c r="E182" s="17"/>
-      <c r="F182" s="17"/>
-      <c r="G182" s="17"/>
-      <c r="H182" s="17"/>
-      <c r="I182" s="17"/>
-      <c r="J182" s="17"/>
-      <c r="K182" s="17"/>
-      <c r="L182" s="17"/>
-      <c r="M182" s="17"/>
-      <c r="N182" s="17"/>
-      <c r="O182" s="17"/>
-      <c r="P182" s="17"/>
-      <c r="Q182" s="17"/>
-      <c r="R182" s="23"/>
-      <c r="S182" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="T182" s="24"/>
+        <v>191</v>
+      </c>
+      <c r="B182" s="7"/>
+      <c r="C182" s="7"/>
+      <c r="D182" s="7"/>
+      <c r="E182" s="7"/>
+      <c r="F182" s="7"/>
+      <c r="G182" s="7"/>
+      <c r="H182" s="7"/>
+      <c r="I182" s="8"/>
+      <c r="J182" s="8"/>
+      <c r="K182" s="8"/>
+      <c r="L182" s="8"/>
+      <c r="M182" s="8"/>
+      <c r="N182" s="8"/>
+      <c r="O182" s="8"/>
+      <c r="P182" s="8"/>
+      <c r="Q182" s="8"/>
+      <c r="R182" s="26"/>
+      <c r="S182" s="22"/>
+      <c r="T182" s="27"/>
     </row>
     <row r="183" spans="1:20">
       <c r="A183" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B183" s="12"/>
-      <c r="C183" s="12"/>
-      <c r="D183" s="12"/>
-      <c r="E183" s="12"/>
-      <c r="F183" s="12"/>
-      <c r="G183" s="12"/>
-      <c r="H183" s="12"/>
-      <c r="I183" s="12"/>
-      <c r="J183" s="12"/>
-      <c r="K183" s="12"/>
-      <c r="L183" s="12"/>
-      <c r="M183" s="12"/>
-      <c r="N183" s="12"/>
-      <c r="O183" s="12"/>
-      <c r="P183" s="12"/>
-      <c r="Q183" s="12"/>
-      <c r="R183" s="37" t="s">
-        <v>171</v>
-      </c>
-      <c r="S183" s="35"/>
-      <c r="T183" s="24"/>
+        <v>192</v>
+      </c>
+      <c r="B183" s="17"/>
+      <c r="C183" s="17"/>
+      <c r="D183" s="17"/>
+      <c r="E183" s="17"/>
+      <c r="F183" s="17"/>
+      <c r="G183" s="17"/>
+      <c r="H183" s="17"/>
+      <c r="I183" s="17"/>
+      <c r="J183" s="17"/>
+      <c r="K183" s="17"/>
+      <c r="L183" s="17"/>
+      <c r="M183" s="17"/>
+      <c r="N183" s="17"/>
+      <c r="O183" s="17"/>
+      <c r="P183" s="17"/>
+      <c r="Q183" s="17"/>
+      <c r="R183" s="26"/>
+      <c r="S183" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="T183" s="27"/>
     </row>
     <row r="184" spans="1:20">
       <c r="A184" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B184" s="12"/>
       <c r="C184" s="12"/>
@@ -9277,13 +9307,15 @@
       <c r="O184" s="12"/>
       <c r="P184" s="12"/>
       <c r="Q184" s="12"/>
-      <c r="R184" s="38"/>
-      <c r="S184" s="35"/>
-      <c r="T184" s="24"/>
+      <c r="R184" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="S184" s="23"/>
+      <c r="T184" s="27"/>
     </row>
     <row r="185" spans="1:20">
       <c r="A185" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B185" s="12"/>
       <c r="C185" s="12"/>
@@ -9301,13 +9333,13 @@
       <c r="O185" s="12"/>
       <c r="P185" s="12"/>
       <c r="Q185" s="12"/>
-      <c r="R185" s="38"/>
-      <c r="S185" s="35"/>
-      <c r="T185" s="24"/>
+      <c r="R185" s="40"/>
+      <c r="S185" s="23"/>
+      <c r="T185" s="27"/>
     </row>
     <row r="186" spans="1:20">
       <c r="A186" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B186" s="12"/>
       <c r="C186" s="12"/>
@@ -9325,13 +9357,13 @@
       <c r="O186" s="12"/>
       <c r="P186" s="12"/>
       <c r="Q186" s="12"/>
-      <c r="R186" s="38"/>
-      <c r="S186" s="35"/>
-      <c r="T186" s="24"/>
+      <c r="R186" s="40"/>
+      <c r="S186" s="23"/>
+      <c r="T186" s="27"/>
     </row>
     <row r="187" spans="1:20">
       <c r="A187" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B187" s="12"/>
       <c r="C187" s="12"/>
@@ -9349,13 +9381,13 @@
       <c r="O187" s="12"/>
       <c r="P187" s="12"/>
       <c r="Q187" s="12"/>
-      <c r="R187" s="38"/>
-      <c r="S187" s="35"/>
-      <c r="T187" s="24"/>
+      <c r="R187" s="40"/>
+      <c r="S187" s="23"/>
+      <c r="T187" s="27"/>
     </row>
     <row r="188" spans="1:20">
       <c r="A188" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B188" s="12"/>
       <c r="C188" s="12"/>
@@ -9373,13 +9405,13 @@
       <c r="O188" s="12"/>
       <c r="P188" s="12"/>
       <c r="Q188" s="12"/>
-      <c r="R188" s="38"/>
-      <c r="S188" s="35"/>
-      <c r="T188" s="24"/>
+      <c r="R188" s="40"/>
+      <c r="S188" s="23"/>
+      <c r="T188" s="27"/>
     </row>
     <row r="189" spans="1:20">
       <c r="A189" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B189" s="12"/>
       <c r="C189" s="12"/>
@@ -9397,13 +9429,13 @@
       <c r="O189" s="12"/>
       <c r="P189" s="12"/>
       <c r="Q189" s="12"/>
-      <c r="R189" s="38"/>
-      <c r="S189" s="35"/>
-      <c r="T189" s="24"/>
+      <c r="R189" s="40"/>
+      <c r="S189" s="23"/>
+      <c r="T189" s="27"/>
     </row>
     <row r="190" spans="1:20">
       <c r="A190" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B190" s="12"/>
       <c r="C190" s="12"/>
@@ -9421,41 +9453,37 @@
       <c r="O190" s="12"/>
       <c r="P190" s="12"/>
       <c r="Q190" s="12"/>
-      <c r="R190" s="39"/>
-      <c r="S190" s="35"/>
-      <c r="T190" s="24"/>
+      <c r="R190" s="40"/>
+      <c r="S190" s="23"/>
+      <c r="T190" s="27"/>
     </row>
     <row r="191" spans="1:20">
       <c r="A191" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B191" s="14"/>
-      <c r="C191" s="14"/>
-      <c r="D191" s="14"/>
-      <c r="E191" s="14"/>
-      <c r="F191" s="14"/>
-      <c r="G191" s="14"/>
-      <c r="H191" s="14"/>
-      <c r="I191" s="14"/>
-      <c r="J191" s="14"/>
-      <c r="K191" s="14"/>
-      <c r="L191" s="14"/>
-      <c r="M191" s="14"/>
-      <c r="N191" s="14"/>
-      <c r="O191" s="14"/>
-      <c r="P191" s="14"/>
-      <c r="Q191" s="14"/>
-      <c r="R191" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S191" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="T191" s="24"/>
+        <v>200</v>
+      </c>
+      <c r="B191" s="12"/>
+      <c r="C191" s="12"/>
+      <c r="D191" s="12"/>
+      <c r="E191" s="12"/>
+      <c r="F191" s="12"/>
+      <c r="G191" s="12"/>
+      <c r="H191" s="12"/>
+      <c r="I191" s="12"/>
+      <c r="J191" s="12"/>
+      <c r="K191" s="12"/>
+      <c r="L191" s="12"/>
+      <c r="M191" s="12"/>
+      <c r="N191" s="12"/>
+      <c r="O191" s="12"/>
+      <c r="P191" s="12"/>
+      <c r="Q191" s="12"/>
+      <c r="R191" s="41"/>
+      <c r="S191" s="23"/>
+      <c r="T191" s="27"/>
     </row>
     <row r="192" spans="1:20">
       <c r="A192" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B192" s="14"/>
       <c r="C192" s="14"/>
@@ -9474,107 +9502,114 @@
       <c r="P192" s="14"/>
       <c r="Q192" s="14"/>
       <c r="R192" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="S192" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T192" s="24"/>
+      <c r="T192" s="27"/>
     </row>
     <row r="193" spans="1:21">
       <c r="A193" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="B193" s="6"/>
-      <c r="C193" s="6"/>
-      <c r="D193" s="6"/>
-      <c r="E193" s="6"/>
-      <c r="F193" s="6"/>
-      <c r="G193" s="6"/>
-      <c r="H193" s="6"/>
-      <c r="I193" s="6"/>
-      <c r="J193" s="6"/>
-      <c r="K193" s="6"/>
-      <c r="L193" s="6"/>
-      <c r="M193" s="6"/>
-      <c r="N193" s="6"/>
-      <c r="O193" s="6"/>
-      <c r="P193" s="6"/>
-      <c r="Q193" s="16"/>
+        <v>202</v>
+      </c>
+      <c r="B193" s="14"/>
+      <c r="C193" s="14"/>
+      <c r="D193" s="14"/>
+      <c r="E193" s="14"/>
+      <c r="F193" s="14"/>
+      <c r="G193" s="14"/>
+      <c r="H193" s="14"/>
+      <c r="I193" s="14"/>
+      <c r="J193" s="14"/>
+      <c r="K193" s="14"/>
+      <c r="L193" s="14"/>
+      <c r="M193" s="14"/>
+      <c r="N193" s="14"/>
+      <c r="O193" s="14"/>
+      <c r="P193" s="14"/>
+      <c r="Q193" s="14"/>
       <c r="R193" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S193" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="T193" s="24"/>
-      <c r="U193" t="s">
-        <v>28</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="T193" s="27"/>
     </row>
     <row r="194" spans="1:21">
       <c r="A194" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="B194" s="6"/>
-      <c r="C194" s="6"/>
-      <c r="D194" s="6"/>
-      <c r="E194" s="6"/>
-      <c r="F194" s="6"/>
-      <c r="G194" s="6"/>
-      <c r="H194" s="6"/>
-      <c r="I194" s="6"/>
-      <c r="J194" s="6"/>
-      <c r="K194" s="6"/>
-      <c r="L194" s="6"/>
-      <c r="M194" s="6"/>
-      <c r="N194" s="6"/>
-      <c r="O194" s="6"/>
-      <c r="P194" s="6"/>
-      <c r="Q194" s="16"/>
-      <c r="R194" s="6" t="s">
-        <v>27</v>
+        <v>206</v>
+      </c>
+      <c r="B194" s="25"/>
+      <c r="C194" s="25"/>
+      <c r="D194" s="25"/>
+      <c r="E194" s="25"/>
+      <c r="F194" s="25"/>
+      <c r="G194" s="25"/>
+      <c r="H194" s="25"/>
+      <c r="I194" s="25"/>
+      <c r="J194" s="25"/>
+      <c r="K194" s="25"/>
+      <c r="L194" s="25"/>
+      <c r="M194" s="25"/>
+      <c r="N194" s="25"/>
+      <c r="O194" s="25"/>
+      <c r="P194" s="25"/>
+      <c r="Q194" s="25"/>
+      <c r="R194" s="24" t="s">
+        <v>207</v>
       </c>
       <c r="S194" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="T194" s="24"/>
-      <c r="U194" t="s">
-        <v>30</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="T194" s="27"/>
     </row>
     <row r="195" spans="1:21">
       <c r="A195" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B195" s="6"/>
-      <c r="C195" s="6"/>
-      <c r="D195" s="6"/>
-      <c r="E195" s="6"/>
-      <c r="F195" s="6"/>
-      <c r="G195" s="6"/>
-      <c r="H195" s="6"/>
-      <c r="I195" s="6"/>
-      <c r="J195" s="6"/>
-      <c r="K195" s="6"/>
-      <c r="L195" s="6"/>
-      <c r="M195" s="6"/>
-      <c r="N195" s="6"/>
-      <c r="O195" s="6"/>
-      <c r="P195" s="6"/>
-      <c r="Q195" s="16"/>
-      <c r="R195" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S195" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="T195" s="24"/>
-      <c r="U195" t="s">
-        <v>32</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="B195" s="12"/>
+      <c r="C195" s="12"/>
+      <c r="D195" s="12"/>
+      <c r="E195" s="12"/>
+      <c r="F195" s="12"/>
+      <c r="G195" s="12"/>
+      <c r="H195" s="12"/>
+      <c r="I195" s="12"/>
+      <c r="J195" s="12"/>
+      <c r="K195" s="12"/>
+      <c r="L195" s="12"/>
+      <c r="M195" s="12"/>
+      <c r="N195" s="12"/>
+      <c r="O195" s="12"/>
+      <c r="P195" s="12"/>
+      <c r="Q195" s="12"/>
+      <c r="R195" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="S195" s="22"/>
+      <c r="T195" s="27"/>
     </row>
     <row r="196" spans="1:21">
+      <c r="A196" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B196" s="6"/>
+      <c r="C196" s="6"/>
+      <c r="D196" s="6"/>
+      <c r="E196" s="6"/>
+      <c r="F196" s="6"/>
+      <c r="G196" s="6"/>
+      <c r="H196" s="6"/>
+      <c r="I196" s="6"/>
+      <c r="J196" s="6"/>
+      <c r="K196" s="6"/>
+      <c r="L196" s="6"/>
+      <c r="M196" s="6"/>
+      <c r="N196" s="6"/>
+      <c r="O196" s="6"/>
+      <c r="P196" s="6"/>
       <c r="Q196" s="16"/>
       <c r="R196" s="6" t="s">
         <v>27</v>
@@ -9582,8 +9617,83 @@
       <c r="S196" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T196" s="24"/>
+      <c r="T196" s="27"/>
       <c r="U196" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="197" spans="1:21">
+      <c r="A197" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B197" s="6"/>
+      <c r="C197" s="6"/>
+      <c r="D197" s="6"/>
+      <c r="E197" s="6"/>
+      <c r="F197" s="6"/>
+      <c r="G197" s="6"/>
+      <c r="H197" s="6"/>
+      <c r="I197" s="6"/>
+      <c r="J197" s="6"/>
+      <c r="K197" s="6"/>
+      <c r="L197" s="6"/>
+      <c r="M197" s="6"/>
+      <c r="N197" s="6"/>
+      <c r="O197" s="6"/>
+      <c r="P197" s="6"/>
+      <c r="Q197" s="16"/>
+      <c r="R197" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S197" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="T197" s="27"/>
+      <c r="U197" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="198" spans="1:21">
+      <c r="A198" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B198" s="6"/>
+      <c r="C198" s="6"/>
+      <c r="D198" s="6"/>
+      <c r="E198" s="6"/>
+      <c r="F198" s="6"/>
+      <c r="G198" s="6"/>
+      <c r="H198" s="6"/>
+      <c r="I198" s="6"/>
+      <c r="J198" s="6"/>
+      <c r="K198" s="6"/>
+      <c r="L198" s="6"/>
+      <c r="M198" s="6"/>
+      <c r="N198" s="6"/>
+      <c r="O198" s="6"/>
+      <c r="P198" s="6"/>
+      <c r="Q198" s="16"/>
+      <c r="R198" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S198" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="T198" s="27"/>
+      <c r="U198" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="199" spans="1:21">
+      <c r="Q199" s="16"/>
+      <c r="R199" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S199" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="T199" s="27"/>
+      <c r="U199" t="s">
         <v>34</v>
       </c>
     </row>
@@ -9591,11 +9701,11 @@
   <mergeCells count="25">
     <mergeCell ref="R158:R165"/>
     <mergeCell ref="U158:V158"/>
-    <mergeCell ref="T158:T171"/>
-    <mergeCell ref="R175:R182"/>
-    <mergeCell ref="T175:T196"/>
-    <mergeCell ref="U175:V175"/>
-    <mergeCell ref="R183:R190"/>
+    <mergeCell ref="T158:T172"/>
+    <mergeCell ref="R176:R183"/>
+    <mergeCell ref="T176:T199"/>
+    <mergeCell ref="U176:V176"/>
+    <mergeCell ref="R184:R191"/>
     <mergeCell ref="R4:R11"/>
     <mergeCell ref="T11:T17"/>
     <mergeCell ref="R21:R28"/>

</xml_diff>